<commit_message>
Update the scripts and relevant test data to make the script: TS_NGQ_CPQ_EncoreRetirement_US9408_SearchBundlesWithoutCustomerInformationEntered_01 works fine
</commit_message>
<xml_diff>
--- a/data/TD_NGQ_CPQ_EncoreRetirement_US9408_SearchBundlesWithoutCustomerInformationEntered_01.xlsx
+++ b/data/TD_NGQ_CPQ_EncoreRetirement_US9408_SearchBundlesWithoutCustomerInformationEntered_01.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huntejos\NGQ\NGQ\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2040" windowWidth="23040" windowHeight="8985"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>QuotaName</t>
   </si>
@@ -35,7 +30,13 @@
     <t>BundleID</t>
   </si>
   <si>
-    <t>EB000042</t>
+    <t>EB000016</t>
+  </si>
+  <si>
+    <t>OpportunityID</t>
+  </si>
+  <si>
+    <t>OPE-0002907630</t>
   </si>
 </sst>
 </file>
@@ -345,7 +346,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -353,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -365,20 +366,26 @@
     <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test datat for US9408_01 and function: LineItemDetails_AddProductByNumber
</commit_message>
<xml_diff>
--- a/data/TD_NGQ_CPQ_EncoreRetirement_US9408_SearchBundlesWithoutCustomerInformationEntered_01.xlsx
+++ b/data/TD_NGQ_CPQ_EncoreRetirement_US9408_SearchBundlesWithoutCustomerInformationEntered_01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>QuotaName</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>OPE-0002907630</t>
+  </si>
+  <si>
+    <t>EB000013</t>
   </si>
 </sst>
 </file>
@@ -346,7 +349,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -354,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,10 +385,15 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retrofit US9400_08,US9408_01 and US9408_02
</commit_message>
<xml_diff>
--- a/data/TD_NGQ_CPQ_EncoreRetirement_US9408_SearchBundlesWithoutCustomerInformationEntered_01.xlsx
+++ b/data/TD_NGQ_CPQ_EncoreRetirement_US9408_SearchBundlesWithoutCustomerInformationEntered_01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>QuotaName</t>
   </si>
@@ -30,29 +30,53 @@
     <t>BundleID</t>
   </si>
   <si>
-    <t>EB000016</t>
-  </si>
-  <si>
     <t>OpportunityID</t>
   </si>
   <si>
     <t>OPE-0002907630</t>
   </si>
   <si>
-    <t>EB000013</t>
+    <t>EB001250</t>
+  </si>
+  <si>
+    <t>productNum</t>
+  </si>
+  <si>
+    <t>productDesc</t>
+  </si>
+  <si>
+    <t>productOpt</t>
+  </si>
+  <si>
+    <t>H1K92A3</t>
+  </si>
+  <si>
+    <t>HPE 3Y Proactive Care 24x7 SVC</t>
+  </si>
+  <si>
+    <t>HP Install DL36x(p) Service</t>
+  </si>
+  <si>
+    <t>U4506E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,7 +374,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -357,19 +382,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -377,26 +406,45 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>3</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>